<commit_message>
examples for multiple and diamond inheritance
</commit_message>
<xml_diff>
--- a/Examples/reposit/complex/ComplexLibXL/Workbooks/AddinXl.xlsx
+++ b/Examples/reposit/complex/ComplexLibXL/Workbooks/AddinXl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>coercions</t>
   </si>
@@ -73,6 +73,54 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>multiple inheritance:</t>
+  </si>
+  <si>
+    <t>create a FooBar</t>
+  </si>
+  <si>
+    <t>use it as a Foo</t>
+  </si>
+  <si>
+    <t>use it as a Bar</t>
+  </si>
+  <si>
+    <t>diamond inheritance:</t>
+  </si>
+  <si>
+    <t>create a Foo2</t>
+  </si>
+  <si>
+    <t>create a Bar2</t>
+  </si>
+  <si>
+    <t>create a FooBar2</t>
+  </si>
+  <si>
+    <t>use foo2 as a Foo2</t>
+  </si>
+  <si>
+    <t>use foobar2 as a Foo2</t>
+  </si>
+  <si>
+    <t>use bar2 as a Bar2</t>
+  </si>
+  <si>
+    <t>use foobar2 as a Bar2</t>
+  </si>
+  <si>
+    <t>call Foo2::f() on foo2</t>
+  </si>
+  <si>
+    <t>call Foo2::f() on foobar2</t>
+  </si>
+  <si>
+    <t>call Bar2::f() on bar2</t>
+  </si>
+  <si>
+    <t>call Bar2::f() on foobar2</t>
   </si>
 </sst>
 </file>
@@ -415,7 +463,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -722,6 +770,142 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C39" t="e">
         <f ca="1">_xll.clTest2F(,C38)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="e">
+        <f ca="1">_xll.clFooBar(,"foobar")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" t="e">
+        <f ca="1">_xll.clFunctionUsingFoo(,C41)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" t="e">
+        <f ca="1">_xll.clFunctionUsingBar(,C41)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" t="e">
+        <f ca="1">_xll.clFoo2(,"foo2")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" t="e">
+        <f ca="1">_xll.clBar2(,"bar2")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" t="e">
+        <f ca="1">_xll.clFooBar2(,"foobar2")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="e">
+        <f ca="1">_xll.clFoo2F(,C45)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" t="e">
+        <f ca="1">_xll.clFoo2F(,C47)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" t="e">
+        <f ca="1">_xll.clBar2F(,C46)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" t="e">
+        <f ca="1">_xll.clBar2F(,C47)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" t="e">
+        <f ca="1">_xll.clFunctionUsingFoo2(,C45)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" t="e">
+        <f ca="1">_xll.clFunctionUsingFoo2(,C47)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" t="e">
+        <f ca="1">_xll.clFunctionUsingBar2(,C46)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55" t="e">
+        <f ca="1">_xll.clFunctionUsingBar2(,C47)</f>
         <v>#NAME?</v>
       </c>
     </row>

</xml_diff>